<commit_message>
added inputs for attic and crawl vents. calibrating EFAF HEMS models.
</commit_message>
<xml_diff>
--- a/Projects/EFAF_1921_Annual_Iter_3/RunReport_EFAF_1921_Annual_Iter_3.xlsx
+++ b/Projects/EFAF_1921_Annual_Iter_3/RunReport_EFAF_1921_Annual_Iter_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Repositories\REEDR\Projects\EFAF_1921_Annual_Iter_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F85BC5-EEAA-4B01-BB4E-6BE79BDB78F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874C9408-1EB3-4E4D-A935-45CE6501238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model Out" sheetId="1" r:id="rId1"/>
@@ -20419,7 +20419,7 @@
   <dimension ref="A1:AO24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>